<commit_message>
Input validator added to validate inputs
</commit_message>
<xml_diff>
--- a/resources/BookMyShow.xlsx
+++ b/resources/BookMyShow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbhurtel\PycharmProjects\PythonTrack_HU\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbhurtel\PycharmProjects\PythonAndPytest\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F4DD4-9E1F-45E5-BE6A-7E8C489B3C16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B712CB29-C4E2-43C7-B5C5-8A12105DCA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="2630" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{129A9AA1-7AC5-46DF-83D3-F055B7B02343}"/>
+    <workbookView xWindow="1360" yWindow="2370" windowWidth="14400" windowHeight="7360" xr2:uid="{129A9AA1-7AC5-46DF-83D3-F055B7B02343}"/>
   </bookViews>
   <sheets>
     <sheet name="UserDetails" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
   <si>
     <t>Title</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Director</t>
   </si>
   <si>
-    <t>Admin Rating</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -89,62 +86,188 @@
     <t>Show</t>
   </si>
   <si>
+    <t>First show</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>ef</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>2h 30m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raja mouli </t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>8h 0m</t>
+  </si>
+  <si>
+    <t>0h 30m</t>
+  </si>
+  <si>
+    <t>0h 45m</t>
+  </si>
+  <si>
+    <t>RRR14</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:25</t>
+  </si>
+  <si>
+    <t>RRR15</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:26</t>
+  </si>
+  <si>
+    <t>RRR16</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:27</t>
+  </si>
+  <si>
+    <t>RRR18</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:29</t>
+  </si>
+  <si>
+    <t>RRR19</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:30</t>
+  </si>
+  <si>
+    <t>RRR20</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:31</t>
+  </si>
+  <si>
+    <t>RRR21</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:32</t>
+  </si>
+  <si>
+    <t>RRR22</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:33</t>
+  </si>
+  <si>
+    <t>RRR23</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:34</t>
+  </si>
+  <si>
+    <t>RRR24</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:35</t>
+  </si>
+  <si>
+    <t>RRR25</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:36</t>
+  </si>
+  <si>
+    <t>RRR26</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:37</t>
+  </si>
+  <si>
+    <t>RRR27</t>
+  </si>
+  <si>
+    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:38</t>
+  </si>
+  <si>
     <t>Test</t>
   </si>
   <si>
-    <t>First show</t>
-  </si>
-  <si>
-    <t>8h 0m</t>
-  </si>
-  <si>
-    <t>0h 30m</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>ef</t>
-  </si>
-  <si>
-    <t>dsf</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>User1</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>RRR</t>
-  </si>
-  <si>
-    <t>2h 30m</t>
-  </si>
-  <si>
-    <t>NTR</t>
-  </si>
-  <si>
-    <t>0h 45m</t>
-  </si>
-  <si>
-    <t>8:0-11:0 11:45-14:45 15:30-18:30 19:15-22:15</t>
+    <t>90m</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>8h 40m</t>
+  </si>
+  <si>
+    <t>40m</t>
+  </si>
+  <si>
+    <t>8:40-10:50 11:30-13:40 14:20-16:30 17:10-19:20</t>
+  </si>
+  <si>
+    <t>1h 20m</t>
+  </si>
+  <si>
+    <t>Eng</t>
+  </si>
+  <si>
+    <t>8h 00m</t>
+  </si>
+  <si>
+    <t>20m</t>
+  </si>
+  <si>
+    <t>8:0-10:0 10:20-12:20 12:40-14:40 15:0-17:0</t>
+  </si>
+  <si>
+    <t>Admin Rating(1-10)</t>
+  </si>
+  <si>
+    <t>1h 30m</t>
+  </si>
+  <si>
+    <t>9h 40m</t>
+  </si>
+  <si>
+    <t>9:40-11:50 12:10-14:20 14:40-16:50 17:10-19:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,10 +276,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF808080"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,11 +302,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,11 +620,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869839AA-D17B-4083-B1F5-5C8BFB9C303D}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
@@ -513,55 +633,55 @@
     <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -572,15 +692,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7533FBE8-7CFD-4325-A061-660BCA8F97E3}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,72 +732,688 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" t="s">
+        <v>32</v>
+      </c>
+      <c r="L14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16">
+        <v>4.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2">
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="I17" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17">
         <v>400</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -672,26 +1423,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009FC624-CC77-4259-9D51-0F07A8D6C9D0}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>